<commit_message>
sobel method added onto edge_detection modeule
</commit_message>
<xml_diff>
--- a/Gannt chart 2020.xlsx
+++ b/Gannt chart 2020.xlsx
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="163">
   <si>
     <t>WBS</t>
   </si>
@@ -1562,25 +1562,10 @@
     <t>Impove Well Detection</t>
   </si>
   <si>
-    <t>2.1.1</t>
-  </si>
-  <si>
-    <t>2.1.2</t>
-  </si>
-  <si>
     <t>Automate Plate Cropping</t>
   </si>
   <si>
     <t>Impove Well Centroid Locating</t>
-  </si>
-  <si>
-    <t>Reduce Fisheye Effect</t>
-  </si>
-  <si>
-    <t>2.1.3</t>
-  </si>
-  <si>
-    <t>Test Fisheye</t>
   </si>
   <si>
     <t>Test Well Centroid</t>
@@ -2962,6 +2947,24 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2969,27 +2972,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3166,7 +3151,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="2"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3189,7 +3174,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3253,7 +3238,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3303,7 +3288,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3387,7 +3372,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3442,7 +3427,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3497,7 +3482,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3822,11 +3807,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN38"/>
+  <dimension ref="A1:BN36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3846,7 +3831,7 @@
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="123" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -3854,33 +3839,33 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="I1" s="130"/>
-      <c r="K1" s="162" t="s">
+      <c r="K1" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="168"/>
+      <c r="W1" s="168"/>
+      <c r="X1" s="168"/>
+      <c r="Y1" s="168"/>
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="168"/>
+      <c r="AB1" s="168"/>
+      <c r="AC1" s="168"/>
+      <c r="AD1" s="168"/>
+      <c r="AE1" s="168"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3921,194 +3906,194 @@
       <c r="B4" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="170">
         <v>43920</v>
       </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="109"/>
       <c r="G4" s="112" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="110"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="164" t="str">
+      <c r="K4" s="162" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 1</v>
-      </c>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165"/>
-      <c r="N4" s="165"/>
-      <c r="O4" s="165"/>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="166"/>
-      <c r="R4" s="164" t="str">
+        <v>Week 2</v>
+      </c>
+      <c r="L4" s="163"/>
+      <c r="M4" s="163"/>
+      <c r="N4" s="163"/>
+      <c r="O4" s="163"/>
+      <c r="P4" s="163"/>
+      <c r="Q4" s="164"/>
+      <c r="R4" s="162" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 2</v>
-      </c>
-      <c r="S4" s="165"/>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165"/>
-      <c r="V4" s="165"/>
-      <c r="W4" s="165"/>
-      <c r="X4" s="166"/>
-      <c r="Y4" s="164" t="str">
+        <v>Week 3</v>
+      </c>
+      <c r="S4" s="163"/>
+      <c r="T4" s="163"/>
+      <c r="U4" s="163"/>
+      <c r="V4" s="163"/>
+      <c r="W4" s="163"/>
+      <c r="X4" s="164"/>
+      <c r="Y4" s="162" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 3</v>
-      </c>
-      <c r="Z4" s="165"/>
-      <c r="AA4" s="165"/>
-      <c r="AB4" s="165"/>
-      <c r="AC4" s="165"/>
-      <c r="AD4" s="165"/>
-      <c r="AE4" s="166"/>
-      <c r="AF4" s="164" t="str">
+        <v>Week 4</v>
+      </c>
+      <c r="Z4" s="163"/>
+      <c r="AA4" s="163"/>
+      <c r="AB4" s="163"/>
+      <c r="AC4" s="163"/>
+      <c r="AD4" s="163"/>
+      <c r="AE4" s="164"/>
+      <c r="AF4" s="162" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 4</v>
-      </c>
-      <c r="AG4" s="165"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165"/>
-      <c r="AJ4" s="165"/>
-      <c r="AK4" s="165"/>
-      <c r="AL4" s="166"/>
-      <c r="AM4" s="164" t="str">
+        <v>Week 5</v>
+      </c>
+      <c r="AG4" s="163"/>
+      <c r="AH4" s="163"/>
+      <c r="AI4" s="163"/>
+      <c r="AJ4" s="163"/>
+      <c r="AK4" s="163"/>
+      <c r="AL4" s="164"/>
+      <c r="AM4" s="162" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="AN4" s="165"/>
-      <c r="AO4" s="165"/>
-      <c r="AP4" s="165"/>
-      <c r="AQ4" s="165"/>
-      <c r="AR4" s="165"/>
-      <c r="AS4" s="166"/>
-      <c r="AT4" s="164" t="str">
+        <v>Week 6</v>
+      </c>
+      <c r="AN4" s="163"/>
+      <c r="AO4" s="163"/>
+      <c r="AP4" s="163"/>
+      <c r="AQ4" s="163"/>
+      <c r="AR4" s="163"/>
+      <c r="AS4" s="164"/>
+      <c r="AT4" s="162" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="AU4" s="165"/>
-      <c r="AV4" s="165"/>
-      <c r="AW4" s="165"/>
-      <c r="AX4" s="165"/>
-      <c r="AY4" s="165"/>
-      <c r="AZ4" s="166"/>
-      <c r="BA4" s="164" t="str">
+        <v>Week 7</v>
+      </c>
+      <c r="AU4" s="163"/>
+      <c r="AV4" s="163"/>
+      <c r="AW4" s="163"/>
+      <c r="AX4" s="163"/>
+      <c r="AY4" s="163"/>
+      <c r="AZ4" s="164"/>
+      <c r="BA4" s="162" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="BB4" s="165"/>
-      <c r="BC4" s="165"/>
-      <c r="BD4" s="165"/>
-      <c r="BE4" s="165"/>
-      <c r="BF4" s="165"/>
-      <c r="BG4" s="166"/>
-      <c r="BH4" s="164" t="str">
+        <v>Week 8</v>
+      </c>
+      <c r="BB4" s="163"/>
+      <c r="BC4" s="163"/>
+      <c r="BD4" s="163"/>
+      <c r="BE4" s="163"/>
+      <c r="BF4" s="163"/>
+      <c r="BG4" s="164"/>
+      <c r="BH4" s="162" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="BI4" s="165"/>
-      <c r="BJ4" s="165"/>
-      <c r="BK4" s="165"/>
-      <c r="BL4" s="165"/>
-      <c r="BM4" s="165"/>
-      <c r="BN4" s="166"/>
+        <v>Week 9</v>
+      </c>
+      <c r="BI4" s="163"/>
+      <c r="BJ4" s="163"/>
+      <c r="BK4" s="163"/>
+      <c r="BL4" s="163"/>
+      <c r="BM4" s="163"/>
+      <c r="BN4" s="164"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="108"/>
       <c r="B5" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="168">
+      <c r="K5" s="165">
         <f>K6</f>
-        <v>43920</v>
-      </c>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="168">
+        <v>43927</v>
+      </c>
+      <c r="L5" s="166"/>
+      <c r="M5" s="166"/>
+      <c r="N5" s="166"/>
+      <c r="O5" s="166"/>
+      <c r="P5" s="166"/>
+      <c r="Q5" s="167"/>
+      <c r="R5" s="165">
         <f>R6</f>
-        <v>43927</v>
-      </c>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
-      <c r="U5" s="169"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="169"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="168">
+        <v>43934</v>
+      </c>
+      <c r="S5" s="166"/>
+      <c r="T5" s="166"/>
+      <c r="U5" s="166"/>
+      <c r="V5" s="166"/>
+      <c r="W5" s="166"/>
+      <c r="X5" s="167"/>
+      <c r="Y5" s="165">
         <f>Y6</f>
-        <v>43934</v>
-      </c>
-      <c r="Z5" s="169"/>
-      <c r="AA5" s="169"/>
-      <c r="AB5" s="169"/>
-      <c r="AC5" s="169"/>
-      <c r="AD5" s="169"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="168">
+        <v>43941</v>
+      </c>
+      <c r="Z5" s="166"/>
+      <c r="AA5" s="166"/>
+      <c r="AB5" s="166"/>
+      <c r="AC5" s="166"/>
+      <c r="AD5" s="166"/>
+      <c r="AE5" s="167"/>
+      <c r="AF5" s="165">
         <f>AF6</f>
-        <v>43941</v>
-      </c>
-      <c r="AG5" s="169"/>
-      <c r="AH5" s="169"/>
-      <c r="AI5" s="169"/>
-      <c r="AJ5" s="169"/>
-      <c r="AK5" s="169"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="168">
+        <v>43948</v>
+      </c>
+      <c r="AG5" s="166"/>
+      <c r="AH5" s="166"/>
+      <c r="AI5" s="166"/>
+      <c r="AJ5" s="166"/>
+      <c r="AK5" s="166"/>
+      <c r="AL5" s="167"/>
+      <c r="AM5" s="165">
         <f>AM6</f>
-        <v>43948</v>
-      </c>
-      <c r="AN5" s="169"/>
-      <c r="AO5" s="169"/>
-      <c r="AP5" s="169"/>
-      <c r="AQ5" s="169"/>
-      <c r="AR5" s="169"/>
-      <c r="AS5" s="170"/>
-      <c r="AT5" s="168">
+        <v>43955</v>
+      </c>
+      <c r="AN5" s="166"/>
+      <c r="AO5" s="166"/>
+      <c r="AP5" s="166"/>
+      <c r="AQ5" s="166"/>
+      <c r="AR5" s="166"/>
+      <c r="AS5" s="167"/>
+      <c r="AT5" s="165">
         <f>AT6</f>
-        <v>43955</v>
-      </c>
-      <c r="AU5" s="169"/>
-      <c r="AV5" s="169"/>
-      <c r="AW5" s="169"/>
-      <c r="AX5" s="169"/>
-      <c r="AY5" s="169"/>
-      <c r="AZ5" s="170"/>
-      <c r="BA5" s="168">
+        <v>43962</v>
+      </c>
+      <c r="AU5" s="166"/>
+      <c r="AV5" s="166"/>
+      <c r="AW5" s="166"/>
+      <c r="AX5" s="166"/>
+      <c r="AY5" s="166"/>
+      <c r="AZ5" s="167"/>
+      <c r="BA5" s="165">
         <f>BA6</f>
-        <v>43962</v>
-      </c>
-      <c r="BB5" s="169"/>
-      <c r="BC5" s="169"/>
-      <c r="BD5" s="169"/>
-      <c r="BE5" s="169"/>
-      <c r="BF5" s="169"/>
-      <c r="BG5" s="170"/>
-      <c r="BH5" s="168">
+        <v>43969</v>
+      </c>
+      <c r="BB5" s="166"/>
+      <c r="BC5" s="166"/>
+      <c r="BD5" s="166"/>
+      <c r="BE5" s="166"/>
+      <c r="BF5" s="166"/>
+      <c r="BG5" s="167"/>
+      <c r="BH5" s="165">
         <f>BH6</f>
-        <v>43969</v>
-      </c>
-      <c r="BI5" s="169"/>
-      <c r="BJ5" s="169"/>
-      <c r="BK5" s="169"/>
-      <c r="BL5" s="169"/>
-      <c r="BM5" s="169"/>
-      <c r="BN5" s="170"/>
+        <v>43976</v>
+      </c>
+      <c r="BI5" s="166"/>
+      <c r="BJ5" s="166"/>
+      <c r="BK5" s="166"/>
+      <c r="BL5" s="166"/>
+      <c r="BM5" s="166"/>
+      <c r="BN5" s="167"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -4123,227 +4108,227 @@
       <c r="J6" s="49"/>
       <c r="K6" s="91">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="L6" s="82">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43921</v>
+        <v>43928</v>
       </c>
       <c r="M6" s="82">
         <f t="shared" si="0"/>
-        <v>43922</v>
+        <v>43929</v>
       </c>
       <c r="N6" s="82">
         <f t="shared" si="0"/>
-        <v>43923</v>
+        <v>43930</v>
       </c>
       <c r="O6" s="82">
         <f t="shared" si="0"/>
-        <v>43924</v>
+        <v>43931</v>
       </c>
       <c r="P6" s="82">
         <f t="shared" si="0"/>
-        <v>43925</v>
+        <v>43932</v>
       </c>
       <c r="Q6" s="92">
         <f t="shared" si="0"/>
-        <v>43926</v>
+        <v>43933</v>
       </c>
       <c r="R6" s="91">
         <f t="shared" si="0"/>
-        <v>43927</v>
+        <v>43934</v>
       </c>
       <c r="S6" s="82">
         <f t="shared" si="0"/>
-        <v>43928</v>
+        <v>43935</v>
       </c>
       <c r="T6" s="82">
         <f t="shared" si="0"/>
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="U6" s="82">
         <f t="shared" si="0"/>
-        <v>43930</v>
+        <v>43937</v>
       </c>
       <c r="V6" s="82">
         <f t="shared" si="0"/>
-        <v>43931</v>
+        <v>43938</v>
       </c>
       <c r="W6" s="82">
         <f t="shared" si="0"/>
-        <v>43932</v>
+        <v>43939</v>
       </c>
       <c r="X6" s="92">
         <f t="shared" si="0"/>
-        <v>43933</v>
+        <v>43940</v>
       </c>
       <c r="Y6" s="91">
         <f t="shared" si="0"/>
-        <v>43934</v>
+        <v>43941</v>
       </c>
       <c r="Z6" s="82">
         <f t="shared" si="0"/>
-        <v>43935</v>
+        <v>43942</v>
       </c>
       <c r="AA6" s="82">
         <f t="shared" si="0"/>
-        <v>43936</v>
+        <v>43943</v>
       </c>
       <c r="AB6" s="82">
         <f t="shared" si="0"/>
-        <v>43937</v>
+        <v>43944</v>
       </c>
       <c r="AC6" s="82">
         <f t="shared" si="0"/>
-        <v>43938</v>
+        <v>43945</v>
       </c>
       <c r="AD6" s="82">
         <f t="shared" si="0"/>
-        <v>43939</v>
+        <v>43946</v>
       </c>
       <c r="AE6" s="92">
         <f t="shared" si="0"/>
-        <v>43940</v>
+        <v>43947</v>
       </c>
       <c r="AF6" s="91">
         <f t="shared" si="0"/>
-        <v>43941</v>
+        <v>43948</v>
       </c>
       <c r="AG6" s="82">
         <f t="shared" si="0"/>
-        <v>43942</v>
+        <v>43949</v>
       </c>
       <c r="AH6" s="82">
         <f t="shared" si="0"/>
-        <v>43943</v>
+        <v>43950</v>
       </c>
       <c r="AI6" s="82">
         <f t="shared" si="0"/>
-        <v>43944</v>
+        <v>43951</v>
       </c>
       <c r="AJ6" s="82">
         <f t="shared" si="0"/>
-        <v>43945</v>
+        <v>43952</v>
       </c>
       <c r="AK6" s="82">
         <f t="shared" si="0"/>
-        <v>43946</v>
+        <v>43953</v>
       </c>
       <c r="AL6" s="92">
         <f t="shared" si="0"/>
-        <v>43947</v>
+        <v>43954</v>
       </c>
       <c r="AM6" s="91">
         <f t="shared" si="0"/>
-        <v>43948</v>
+        <v>43955</v>
       </c>
       <c r="AN6" s="82">
         <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>43956</v>
       </c>
       <c r="AO6" s="82">
         <f t="shared" si="0"/>
-        <v>43950</v>
+        <v>43957</v>
       </c>
       <c r="AP6" s="82">
         <f t="shared" si="0"/>
-        <v>43951</v>
+        <v>43958</v>
       </c>
       <c r="AQ6" s="82">
         <f t="shared" si="0"/>
-        <v>43952</v>
+        <v>43959</v>
       </c>
       <c r="AR6" s="82">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43953</v>
+        <v>43960</v>
       </c>
       <c r="AS6" s="92">
         <f t="shared" si="1"/>
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="AT6" s="91">
         <f t="shared" si="1"/>
-        <v>43955</v>
+        <v>43962</v>
       </c>
       <c r="AU6" s="82">
         <f t="shared" si="1"/>
-        <v>43956</v>
+        <v>43963</v>
       </c>
       <c r="AV6" s="82">
         <f t="shared" si="1"/>
-        <v>43957</v>
+        <v>43964</v>
       </c>
       <c r="AW6" s="82">
         <f t="shared" si="1"/>
-        <v>43958</v>
+        <v>43965</v>
       </c>
       <c r="AX6" s="82">
         <f t="shared" si="1"/>
-        <v>43959</v>
+        <v>43966</v>
       </c>
       <c r="AY6" s="82">
         <f t="shared" si="1"/>
-        <v>43960</v>
+        <v>43967</v>
       </c>
       <c r="AZ6" s="92">
         <f t="shared" si="1"/>
-        <v>43961</v>
+        <v>43968</v>
       </c>
       <c r="BA6" s="91">
         <f t="shared" si="1"/>
-        <v>43962</v>
+        <v>43969</v>
       </c>
       <c r="BB6" s="82">
         <f t="shared" si="1"/>
-        <v>43963</v>
+        <v>43970</v>
       </c>
       <c r="BC6" s="82">
         <f t="shared" si="1"/>
-        <v>43964</v>
+        <v>43971</v>
       </c>
       <c r="BD6" s="82">
         <f t="shared" si="1"/>
-        <v>43965</v>
+        <v>43972</v>
       </c>
       <c r="BE6" s="82">
         <f t="shared" si="1"/>
-        <v>43966</v>
+        <v>43973</v>
       </c>
       <c r="BF6" s="82">
         <f t="shared" si="1"/>
-        <v>43967</v>
+        <v>43974</v>
       </c>
       <c r="BG6" s="92">
         <f t="shared" si="1"/>
-        <v>43968</v>
+        <v>43975</v>
       </c>
       <c r="BH6" s="91">
         <f t="shared" si="1"/>
-        <v>43969</v>
+        <v>43976</v>
       </c>
       <c r="BI6" s="82">
         <f t="shared" si="1"/>
-        <v>43970</v>
+        <v>43977</v>
       </c>
       <c r="BJ6" s="82">
         <f t="shared" si="1"/>
-        <v>43971</v>
+        <v>43978</v>
       </c>
       <c r="BK6" s="82">
         <f t="shared" si="1"/>
-        <v>43972</v>
+        <v>43979</v>
       </c>
       <c r="BL6" s="82">
         <f t="shared" si="1"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="BM6" s="82">
         <f t="shared" si="1"/>
-        <v>43974</v>
+        <v>43981</v>
       </c>
       <c r="BN6" s="92">
         <f t="shared" si="1"/>
-        <v>43975</v>
+        <v>43982</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="122" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -4618,7 +4603,7 @@
       <c r="G8" s="88"/>
       <c r="H8" s="89"/>
       <c r="I8" s="90" t="str">
-        <f t="shared" ref="I8:I31" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I29" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="93"/>
@@ -4688,7 +4673,7 @@
         <v>145</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D9" s="125"/>
       <c r="E9" s="99">
@@ -4774,7 +4759,7 @@
         <v>146</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D10" s="125"/>
       <c r="E10" s="99">
@@ -4861,7 +4846,7 @@
         <v>147</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D11" s="125"/>
       <c r="E11" s="99">
@@ -4947,7 +4932,7 @@
         <v>148</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D12" s="125"/>
       <c r="E12" s="99">
@@ -5035,7 +5020,7 @@
       <c r="D13" s="55"/>
       <c r="E13" s="101"/>
       <c r="F13" s="101" t="str">
-        <f t="shared" ref="F13:F29" si="6">IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+        <f t="shared" ref="F13:F25" si="6">IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G13" s="56"/>
@@ -5110,6 +5095,9 @@
       <c r="B14" s="124" t="s">
         <v>149</v>
       </c>
+      <c r="C14" s="60" t="s">
+        <v>158</v>
+      </c>
       <c r="D14" s="125"/>
       <c r="E14" s="99">
         <v>43934</v>
@@ -5122,8 +5110,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="62">
-        <f>AVERAGE(H15:H17)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I14" s="63">
         <f t="shared" si="4"/>
@@ -5188,14 +5175,15 @@
       <c r="BN14" s="106"/>
     </row>
     <row r="15" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.2</v>
+      </c>
+      <c r="B15" s="124" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="124" t="s">
-        <v>152</v>
-      </c>
       <c r="C15" s="60" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D15" s="125"/>
       <c r="E15" s="99">
@@ -5274,21 +5262,22 @@
       <c r="BN15" s="106"/>
     </row>
     <row r="16" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.3</v>
+      </c>
+      <c r="B16" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="124" t="s">
-        <v>153</v>
-      </c>
       <c r="C16" s="60" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D16" s="125"/>
       <c r="E16" s="99">
         <v>43938</v>
       </c>
       <c r="F16" s="100">
-        <f t="shared" ref="F16:F18" si="7">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
+        <f t="shared" ref="F16:F17" si="7">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
         <v>43961</v>
       </c>
       <c r="G16" s="61">
@@ -5359,15 +5348,16 @@
       <c r="BM16" s="106"/>
       <c r="BN16" s="106"/>
     </row>
-    <row r="17" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
-        <v>155</v>
+    <row r="17" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.4</v>
       </c>
       <c r="B17" s="124" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D17" s="125"/>
       <c r="E17" s="99">
@@ -5445,181 +5435,180 @@
       <c r="BM17" s="106"/>
       <c r="BN17" s="106"/>
     </row>
-    <row r="18" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.2</v>
-      </c>
-      <c r="B18" s="124" t="s">
-        <v>161</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="125"/>
-      <c r="E18" s="99">
-        <v>43938</v>
-      </c>
-      <c r="F18" s="100">
-        <f t="shared" si="7"/>
-        <v>43961</v>
-      </c>
-      <c r="G18" s="61">
-        <v>24</v>
-      </c>
-      <c r="H18" s="62">
-        <v>0</v>
-      </c>
-      <c r="I18" s="63">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="J18" s="94"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="106"/>
-      <c r="M18" s="106"/>
-      <c r="N18" s="106"/>
-      <c r="O18" s="106"/>
-      <c r="P18" s="106"/>
-      <c r="Q18" s="106"/>
-      <c r="R18" s="106"/>
-      <c r="S18" s="106"/>
-      <c r="T18" s="106"/>
-      <c r="U18" s="106"/>
-      <c r="V18" s="106"/>
-      <c r="W18" s="106"/>
-      <c r="X18" s="106"/>
-      <c r="Y18" s="106"/>
-      <c r="Z18" s="106"/>
-      <c r="AA18" s="106"/>
-      <c r="AB18" s="106"/>
-      <c r="AC18" s="106"/>
-      <c r="AD18" s="106"/>
-      <c r="AE18" s="106"/>
-      <c r="AF18" s="106"/>
-      <c r="AG18" s="106"/>
-      <c r="AH18" s="106"/>
-      <c r="AI18" s="106"/>
-      <c r="AJ18" s="106"/>
-      <c r="AK18" s="106"/>
-      <c r="AL18" s="106"/>
-      <c r="AM18" s="106"/>
-      <c r="AN18" s="106"/>
-      <c r="AO18" s="106"/>
-      <c r="AP18" s="106"/>
-      <c r="AQ18" s="106"/>
-      <c r="AR18" s="106"/>
-      <c r="AS18" s="106"/>
-      <c r="AT18" s="106"/>
-      <c r="AU18" s="106"/>
-      <c r="AV18" s="106"/>
-      <c r="AW18" s="106"/>
-      <c r="AX18" s="106"/>
-      <c r="AY18" s="106"/>
-      <c r="AZ18" s="106"/>
-      <c r="BA18" s="106"/>
-      <c r="BB18" s="106"/>
-      <c r="BC18" s="106"/>
-      <c r="BD18" s="106"/>
-      <c r="BE18" s="106"/>
-      <c r="BF18" s="106"/>
-      <c r="BG18" s="106"/>
-      <c r="BH18" s="106"/>
-      <c r="BI18" s="106"/>
-      <c r="BJ18" s="106"/>
-      <c r="BK18" s="106"/>
-      <c r="BL18" s="106"/>
-      <c r="BM18" s="106"/>
-      <c r="BN18" s="106"/>
-    </row>
-    <row r="19" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="52" t="str">
+    <row r="18" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B18" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="55"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101" t="str">
+      <c r="D18" s="55"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G19" s="56"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58" t="str">
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J19" s="95"/>
-      <c r="K19" s="107"/>
-      <c r="L19" s="107"/>
-      <c r="M19" s="107"/>
-      <c r="N19" s="107"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="107"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="107"/>
-      <c r="S19" s="107"/>
-      <c r="T19" s="107"/>
-      <c r="U19" s="107"/>
-      <c r="V19" s="107"/>
-      <c r="W19" s="107"/>
-      <c r="X19" s="107"/>
-      <c r="Y19" s="107"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="107"/>
-      <c r="AB19" s="107"/>
-      <c r="AC19" s="107"/>
-      <c r="AD19" s="107"/>
-      <c r="AE19" s="107"/>
-      <c r="AF19" s="107"/>
-      <c r="AG19" s="107"/>
-      <c r="AH19" s="107"/>
-      <c r="AI19" s="107"/>
-      <c r="AJ19" s="107"/>
-      <c r="AK19" s="107"/>
-      <c r="AL19" s="107"/>
-      <c r="AM19" s="107"/>
-      <c r="AN19" s="107"/>
-      <c r="AO19" s="107"/>
-      <c r="AP19" s="107"/>
-      <c r="AQ19" s="107"/>
-      <c r="AR19" s="107"/>
-      <c r="AS19" s="107"/>
-      <c r="AT19" s="107"/>
-      <c r="AU19" s="107"/>
-      <c r="AV19" s="107"/>
-      <c r="AW19" s="107"/>
-      <c r="AX19" s="107"/>
-      <c r="AY19" s="107"/>
-      <c r="AZ19" s="107"/>
-      <c r="BA19" s="107"/>
-      <c r="BB19" s="107"/>
-      <c r="BC19" s="107"/>
-      <c r="BD19" s="107"/>
-      <c r="BE19" s="107"/>
-      <c r="BF19" s="107"/>
-      <c r="BG19" s="107"/>
-      <c r="BH19" s="107"/>
-      <c r="BI19" s="107"/>
-      <c r="BJ19" s="107"/>
-      <c r="BK19" s="107"/>
-      <c r="BL19" s="107"/>
-      <c r="BM19" s="107"/>
-      <c r="BN19" s="107"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="107"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="107"/>
+      <c r="R18" s="107"/>
+      <c r="S18" s="107"/>
+      <c r="T18" s="107"/>
+      <c r="U18" s="107"/>
+      <c r="V18" s="107"/>
+      <c r="W18" s="107"/>
+      <c r="X18" s="107"/>
+      <c r="Y18" s="107"/>
+      <c r="Z18" s="107"/>
+      <c r="AA18" s="107"/>
+      <c r="AB18" s="107"/>
+      <c r="AC18" s="107"/>
+      <c r="AD18" s="107"/>
+      <c r="AE18" s="107"/>
+      <c r="AF18" s="107"/>
+      <c r="AG18" s="107"/>
+      <c r="AH18" s="107"/>
+      <c r="AI18" s="107"/>
+      <c r="AJ18" s="107"/>
+      <c r="AK18" s="107"/>
+      <c r="AL18" s="107"/>
+      <c r="AM18" s="107"/>
+      <c r="AN18" s="107"/>
+      <c r="AO18" s="107"/>
+      <c r="AP18" s="107"/>
+      <c r="AQ18" s="107"/>
+      <c r="AR18" s="107"/>
+      <c r="AS18" s="107"/>
+      <c r="AT18" s="107"/>
+      <c r="AU18" s="107"/>
+      <c r="AV18" s="107"/>
+      <c r="AW18" s="107"/>
+      <c r="AX18" s="107"/>
+      <c r="AY18" s="107"/>
+      <c r="AZ18" s="107"/>
+      <c r="BA18" s="107"/>
+      <c r="BB18" s="107"/>
+      <c r="BC18" s="107"/>
+      <c r="BD18" s="107"/>
+      <c r="BE18" s="107"/>
+      <c r="BF18" s="107"/>
+      <c r="BG18" s="107"/>
+      <c r="BH18" s="107"/>
+      <c r="BI18" s="107"/>
+      <c r="BJ18" s="107"/>
+      <c r="BK18" s="107"/>
+      <c r="BL18" s="107"/>
+      <c r="BM18" s="107"/>
+      <c r="BN18" s="107"/>
+    </row>
+    <row r="19" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.1</v>
+      </c>
+      <c r="B19" s="124" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="125"/>
+      <c r="E19" s="99">
+        <v>43948</v>
+      </c>
+      <c r="F19" s="100">
+        <v>43968</v>
+      </c>
+      <c r="G19" s="61">
+        <v>3</v>
+      </c>
+      <c r="H19" s="62">
+        <v>0</v>
+      </c>
+      <c r="I19" s="63">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="94"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="106"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="106"/>
+      <c r="P19" s="106"/>
+      <c r="Q19" s="106"/>
+      <c r="R19" s="106"/>
+      <c r="S19" s="106"/>
+      <c r="T19" s="106"/>
+      <c r="U19" s="106"/>
+      <c r="V19" s="106"/>
+      <c r="W19" s="106"/>
+      <c r="X19" s="106"/>
+      <c r="Y19" s="106"/>
+      <c r="Z19" s="106"/>
+      <c r="AA19" s="106"/>
+      <c r="AB19" s="106"/>
+      <c r="AC19" s="106"/>
+      <c r="AD19" s="106"/>
+      <c r="AE19" s="106"/>
+      <c r="AF19" s="106"/>
+      <c r="AG19" s="106"/>
+      <c r="AH19" s="106"/>
+      <c r="AI19" s="106"/>
+      <c r="AJ19" s="106"/>
+      <c r="AK19" s="106"/>
+      <c r="AL19" s="106"/>
+      <c r="AM19" s="106"/>
+      <c r="AN19" s="106"/>
+      <c r="AO19" s="106"/>
+      <c r="AP19" s="106"/>
+      <c r="AQ19" s="106"/>
+      <c r="AR19" s="106"/>
+      <c r="AS19" s="106"/>
+      <c r="AT19" s="106"/>
+      <c r="AU19" s="106"/>
+      <c r="AV19" s="106"/>
+      <c r="AW19" s="106"/>
+      <c r="AX19" s="106"/>
+      <c r="AY19" s="106"/>
+      <c r="AZ19" s="106"/>
+      <c r="BA19" s="106"/>
+      <c r="BB19" s="106"/>
+      <c r="BC19" s="106"/>
+      <c r="BD19" s="106"/>
+      <c r="BE19" s="106"/>
+      <c r="BF19" s="106"/>
+      <c r="BG19" s="106"/>
+      <c r="BH19" s="106"/>
+      <c r="BI19" s="106"/>
+      <c r="BJ19" s="106"/>
+      <c r="BK19" s="106"/>
+      <c r="BL19" s="106"/>
+      <c r="BM19" s="106"/>
+      <c r="BN19" s="106"/>
     </row>
     <row r="20" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="B20" s="124" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D20" s="125"/>
       <c r="E20" s="99">
@@ -5629,7 +5618,7 @@
         <v>43968</v>
       </c>
       <c r="G20" s="61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" s="62">
         <v>0</v>
@@ -5699,13 +5688,13 @@
     <row r="21" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="B21" s="124" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D21" s="125"/>
       <c r="E21" s="99">
@@ -5715,7 +5704,7 @@
         <v>43968</v>
       </c>
       <c r="G21" s="61">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H21" s="62">
         <v>0</v>
@@ -5785,30 +5774,32 @@
     <row r="22" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="B22" s="124" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D22" s="125"/>
       <c r="E22" s="99">
-        <v>43948</v>
+        <f>F14+1</f>
+        <v>43962</v>
       </c>
       <c r="F22" s="100">
+        <f>IF(ISBLANK(E22)," - ",IF(G22=0,E22,E22+G22-1))</f>
         <v>43968</v>
       </c>
       <c r="G22" s="61">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H22" s="62">
         <v>0</v>
       </c>
       <c r="I22" s="63">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J22" s="94"/>
       <c r="K22" s="106"/>
@@ -5868,121 +5859,111 @@
       <c r="BM22" s="106"/>
       <c r="BN22" s="106"/>
     </row>
-    <row r="23" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.4</v>
-      </c>
-      <c r="B23" s="124" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="D23" s="125"/>
-      <c r="E23" s="99">
-        <v>43948</v>
-      </c>
-      <c r="F23" s="100">
-        <v>43968</v>
-      </c>
-      <c r="G23" s="61">
-        <v>6</v>
-      </c>
-      <c r="H23" s="62">
-        <v>0</v>
-      </c>
-      <c r="I23" s="63">
+    <row r="23" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>4</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="55"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="101" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58" t="str">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="J23" s="94"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="106"/>
-      <c r="P23" s="106"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="106"/>
-      <c r="T23" s="106"/>
-      <c r="U23" s="106"/>
-      <c r="V23" s="106"/>
-      <c r="W23" s="106"/>
-      <c r="X23" s="106"/>
-      <c r="Y23" s="106"/>
-      <c r="Z23" s="106"/>
-      <c r="AA23" s="106"/>
-      <c r="AB23" s="106"/>
-      <c r="AC23" s="106"/>
-      <c r="AD23" s="106"/>
-      <c r="AE23" s="106"/>
-      <c r="AF23" s="106"/>
-      <c r="AG23" s="106"/>
-      <c r="AH23" s="106"/>
-      <c r="AI23" s="106"/>
-      <c r="AJ23" s="106"/>
-      <c r="AK23" s="106"/>
-      <c r="AL23" s="106"/>
-      <c r="AM23" s="106"/>
-      <c r="AN23" s="106"/>
-      <c r="AO23" s="106"/>
-      <c r="AP23" s="106"/>
-      <c r="AQ23" s="106"/>
-      <c r="AR23" s="106"/>
-      <c r="AS23" s="106"/>
-      <c r="AT23" s="106"/>
-      <c r="AU23" s="106"/>
-      <c r="AV23" s="106"/>
-      <c r="AW23" s="106"/>
-      <c r="AX23" s="106"/>
-      <c r="AY23" s="106"/>
-      <c r="AZ23" s="106"/>
-      <c r="BA23" s="106"/>
-      <c r="BB23" s="106"/>
-      <c r="BC23" s="106"/>
-      <c r="BD23" s="106"/>
-      <c r="BE23" s="106"/>
-      <c r="BF23" s="106"/>
-      <c r="BG23" s="106"/>
-      <c r="BH23" s="106"/>
-      <c r="BI23" s="106"/>
-      <c r="BJ23" s="106"/>
-      <c r="BK23" s="106"/>
-      <c r="BL23" s="106"/>
-      <c r="BM23" s="106"/>
-      <c r="BN23" s="106"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J23" s="95"/>
+      <c r="K23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
+      <c r="S23" s="107"/>
+      <c r="T23" s="107"/>
+      <c r="U23" s="107"/>
+      <c r="V23" s="107"/>
+      <c r="W23" s="107"/>
+      <c r="X23" s="107"/>
+      <c r="Y23" s="107"/>
+      <c r="Z23" s="107"/>
+      <c r="AA23" s="107"/>
+      <c r="AB23" s="107"/>
+      <c r="AC23" s="107"/>
+      <c r="AD23" s="107"/>
+      <c r="AE23" s="107"/>
+      <c r="AF23" s="107"/>
+      <c r="AG23" s="107"/>
+      <c r="AH23" s="107"/>
+      <c r="AI23" s="107"/>
+      <c r="AJ23" s="107"/>
+      <c r="AK23" s="107"/>
+      <c r="AL23" s="107"/>
+      <c r="AM23" s="107"/>
+      <c r="AN23" s="107"/>
+      <c r="AO23" s="107"/>
+      <c r="AP23" s="107"/>
+      <c r="AQ23" s="107"/>
+      <c r="AR23" s="107"/>
+      <c r="AS23" s="107"/>
+      <c r="AT23" s="107"/>
+      <c r="AU23" s="107"/>
+      <c r="AV23" s="107"/>
+      <c r="AW23" s="107"/>
+      <c r="AX23" s="107"/>
+      <c r="AY23" s="107"/>
+      <c r="AZ23" s="107"/>
+      <c r="BA23" s="107"/>
+      <c r="BB23" s="107"/>
+      <c r="BC23" s="107"/>
+      <c r="BD23" s="107"/>
+      <c r="BE23" s="107"/>
+      <c r="BF23" s="107"/>
+      <c r="BG23" s="107"/>
+      <c r="BH23" s="107"/>
+      <c r="BI23" s="107"/>
+      <c r="BJ23" s="107"/>
+      <c r="BK23" s="107"/>
+      <c r="BL23" s="107"/>
+      <c r="BM23" s="107"/>
+      <c r="BN23" s="107"/>
     </row>
     <row r="24" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.5</v>
+        <v>4.1</v>
       </c>
       <c r="B24" s="124" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D24" s="125"/>
       <c r="E24" s="99">
-        <f>F14+1</f>
-        <v>43962</v>
+        <v>43936</v>
       </c>
       <c r="F24" s="100">
-        <f>IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
-        <v>43968</v>
+        <v>43943</v>
       </c>
       <c r="G24" s="61">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H24" s="62">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I24" s="63">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J24" s="94"/>
       <c r="K24" s="106"/>
@@ -6042,111 +6023,117 @@
       <c r="BM24" s="106"/>
       <c r="BN24" s="106"/>
     </row>
-    <row r="25" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101" t="str">
+    <row r="25" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.2</v>
+      </c>
+      <c r="B25" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="125"/>
+      <c r="E25" s="99">
+        <v>43936</v>
+      </c>
+      <c r="F25" s="100">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G25" s="56"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="58" t="str">
+        <v>43936</v>
+      </c>
+      <c r="G25" s="61">
+        <v>1</v>
+      </c>
+      <c r="H25" s="62">
+        <v>1</v>
+      </c>
+      <c r="I25" s="63">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J25" s="95"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
-      <c r="U25" s="107"/>
-      <c r="V25" s="107"/>
-      <c r="W25" s="107"/>
-      <c r="X25" s="107"/>
-      <c r="Y25" s="107"/>
-      <c r="Z25" s="107"/>
-      <c r="AA25" s="107"/>
-      <c r="AB25" s="107"/>
-      <c r="AC25" s="107"/>
-      <c r="AD25" s="107"/>
-      <c r="AE25" s="107"/>
-      <c r="AF25" s="107"/>
-      <c r="AG25" s="107"/>
-      <c r="AH25" s="107"/>
-      <c r="AI25" s="107"/>
-      <c r="AJ25" s="107"/>
-      <c r="AK25" s="107"/>
-      <c r="AL25" s="107"/>
-      <c r="AM25" s="107"/>
-      <c r="AN25" s="107"/>
-      <c r="AO25" s="107"/>
-      <c r="AP25" s="107"/>
-      <c r="AQ25" s="107"/>
-      <c r="AR25" s="107"/>
-      <c r="AS25" s="107"/>
-      <c r="AT25" s="107"/>
-      <c r="AU25" s="107"/>
-      <c r="AV25" s="107"/>
-      <c r="AW25" s="107"/>
-      <c r="AX25" s="107"/>
-      <c r="AY25" s="107"/>
-      <c r="AZ25" s="107"/>
-      <c r="BA25" s="107"/>
-      <c r="BB25" s="107"/>
-      <c r="BC25" s="107"/>
-      <c r="BD25" s="107"/>
-      <c r="BE25" s="107"/>
-      <c r="BF25" s="107"/>
-      <c r="BG25" s="107"/>
-      <c r="BH25" s="107"/>
-      <c r="BI25" s="107"/>
-      <c r="BJ25" s="107"/>
-      <c r="BK25" s="107"/>
-      <c r="BL25" s="107"/>
-      <c r="BM25" s="107"/>
-      <c r="BN25" s="107"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="94"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
+      <c r="V25" s="106"/>
+      <c r="W25" s="106"/>
+      <c r="X25" s="106"/>
+      <c r="Y25" s="106"/>
+      <c r="Z25" s="106"/>
+      <c r="AA25" s="106"/>
+      <c r="AB25" s="106"/>
+      <c r="AC25" s="106"/>
+      <c r="AD25" s="106"/>
+      <c r="AE25" s="106"/>
+      <c r="AF25" s="106"/>
+      <c r="AG25" s="106"/>
+      <c r="AH25" s="106"/>
+      <c r="AI25" s="106"/>
+      <c r="AJ25" s="106"/>
+      <c r="AK25" s="106"/>
+      <c r="AL25" s="106"/>
+      <c r="AM25" s="106"/>
+      <c r="AN25" s="106"/>
+      <c r="AO25" s="106"/>
+      <c r="AP25" s="106"/>
+      <c r="AQ25" s="106"/>
+      <c r="AR25" s="106"/>
+      <c r="AS25" s="106"/>
+      <c r="AT25" s="106"/>
+      <c r="AU25" s="106"/>
+      <c r="AV25" s="106"/>
+      <c r="AW25" s="106"/>
+      <c r="AX25" s="106"/>
+      <c r="AY25" s="106"/>
+      <c r="AZ25" s="106"/>
+      <c r="BA25" s="106"/>
+      <c r="BB25" s="106"/>
+      <c r="BC25" s="106"/>
+      <c r="BD25" s="106"/>
+      <c r="BE25" s="106"/>
+      <c r="BF25" s="106"/>
+      <c r="BG25" s="106"/>
+      <c r="BH25" s="106"/>
+      <c r="BI25" s="106"/>
+      <c r="BJ25" s="106"/>
+      <c r="BK25" s="106"/>
+      <c r="BL25" s="106"/>
+      <c r="BM25" s="106"/>
+      <c r="BN25" s="106"/>
     </row>
     <row r="26" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
+        <v>4.3</v>
       </c>
       <c r="B26" s="124" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D26" s="125"/>
       <c r="E26" s="99">
-        <v>43936</v>
+        <v>43941</v>
       </c>
       <c r="F26" s="100">
-        <v>43943</v>
+        <v>43992</v>
       </c>
       <c r="G26" s="61">
         <v>1</v>
       </c>
       <c r="H26" s="62">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I26" s="63">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J26" s="94"/>
       <c r="K26" s="106"/>
@@ -6209,28 +6196,30 @@
     <row r="27" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="B27" s="124" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>160</v>
       </c>
       <c r="D27" s="125"/>
       <c r="E27" s="99">
-        <v>43936</v>
+        <v>43941</v>
       </c>
       <c r="F27" s="100">
-        <f t="shared" si="6"/>
-        <v>43936</v>
+        <v>43992</v>
       </c>
       <c r="G27" s="61">
         <v>1</v>
       </c>
       <c r="H27" s="62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="63">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="J27" s="94"/>
       <c r="K27" s="106"/>
@@ -6293,17 +6282,17 @@
     <row r="28" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="B28" s="124" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D28" s="125"/>
       <c r="E28" s="99">
-        <v>43941</v>
+        <v>43983</v>
       </c>
       <c r="F28" s="100">
         <v>43992</v>
@@ -6315,8 +6304,8 @@
         <v>0</v>
       </c>
       <c r="I28" s="63">
-        <f t="shared" si="4"/>
-        <v>38</v>
+        <f t="shared" ref="I28" si="8">IF(OR(F28=0,E28=0)," - ",NETWORKDAYS(E28,F28))</f>
+        <v>8</v>
       </c>
       <c r="J28" s="94"/>
       <c r="K28" s="106"/>
@@ -6376,35 +6365,20 @@
       <c r="BM28" s="106"/>
       <c r="BN28" s="106"/>
     </row>
-    <row r="29" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
-      </c>
-      <c r="B29" s="124" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="99">
-        <v>43941</v>
-      </c>
-      <c r="F29" s="100">
-        <v>43992</v>
-      </c>
-      <c r="G29" s="61">
-        <v>1</v>
-      </c>
-      <c r="H29" s="62">
-        <v>0</v>
-      </c>
-      <c r="I29" s="63">
+    <row r="29" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="59"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68" t="str">
         <f t="shared" si="4"/>
-        <v>38</v>
-      </c>
-      <c r="J29" s="94"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J29" s="96"/>
       <c r="K29" s="106"/>
       <c r="L29" s="106"/>
       <c r="M29" s="106"/>
@@ -6462,35 +6436,19 @@
       <c r="BM29" s="106"/>
       <c r="BN29" s="106"/>
     </row>
-    <row r="30" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
-      </c>
-      <c r="B30" s="124" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="125"/>
-      <c r="E30" s="99">
-        <v>43983</v>
-      </c>
-      <c r="F30" s="100">
-        <v>43992</v>
-      </c>
-      <c r="G30" s="61">
+    <row r="30" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="62">
-        <v>0</v>
-      </c>
-      <c r="I30" s="63">
-        <f t="shared" ref="I30" si="8">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
-        <v>8</v>
-      </c>
-      <c r="J30" s="94"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="97"/>
       <c r="K30" s="106"/>
       <c r="L30" s="106"/>
       <c r="M30" s="106"/>
@@ -6549,19 +6507,18 @@
       <c r="BN30" s="106"/>
     </row>
     <row r="31" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="59"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J31" s="96"/>
+      <c r="A31" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="97"/>
       <c r="K31" s="106"/>
       <c r="L31" s="106"/>
       <c r="M31" s="106"/>
@@ -6619,19 +6576,28 @@
       <c r="BM31" s="106"/>
       <c r="BN31" s="106"/>
     </row>
-    <row r="32" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="70" t="s">
+    <row r="32" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="128" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="97"/>
+      <c r="B32" s="129" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="100" t="str">
+        <f t="shared" ref="F32:F35" si="9">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G32" s="61"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="79" t="str">
+        <f>IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J32" s="98"/>
       <c r="K32" s="106"/>
       <c r="L32" s="106"/>
       <c r="M32" s="106"/>
@@ -6690,18 +6656,27 @@
       <c r="BN32" s="106"/>
     </row>
     <row r="33" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="75" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="104"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="97"/>
+      <c r="A33" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B33" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="80"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="100" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="79" t="str">
+        <f t="shared" ref="I33:I35" si="10">IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J33" s="98"/>
       <c r="K33" s="106"/>
       <c r="L33" s="106"/>
       <c r="M33" s="106"/>
@@ -6760,24 +6735,24 @@
       <c r="BN33" s="106"/>
     </row>
     <row r="34" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="128" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B34" s="129" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="77"/>
+      <c r="A34" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B34" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="80"/>
       <c r="D34" s="78"/>
       <c r="E34" s="99"/>
       <c r="F34" s="100" t="str">
-        <f t="shared" ref="F34:F37" si="9">IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G34" s="61"/>
       <c r="H34" s="62"/>
       <c r="I34" s="79" t="str">
-        <f>IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J34" s="98"/>
@@ -6840,11 +6815,11 @@
     </row>
     <row r="35" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B35" s="80" t="s">
-        <v>62</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>64</v>
       </c>
       <c r="C35" s="80"/>
       <c r="D35" s="78"/>
@@ -6856,7 +6831,7 @@
       <c r="G35" s="61"/>
       <c r="H35" s="62"/>
       <c r="I35" s="79" t="str">
-        <f t="shared" ref="I35:I37" si="10">IF(OR(F35=0,E35=0)," - ",NETWORKDAYS(E35,F35))</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J35" s="98"/>
@@ -6917,238 +6892,89 @@
       <c r="BM35" s="106"/>
       <c r="BN35" s="106"/>
     </row>
-    <row r="36" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B36" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="100" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G36" s="61"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="79" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J36" s="98"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="106"/>
-      <c r="M36" s="106"/>
-      <c r="N36" s="106"/>
-      <c r="O36" s="106"/>
-      <c r="P36" s="106"/>
-      <c r="Q36" s="106"/>
-      <c r="R36" s="106"/>
-      <c r="S36" s="106"/>
-      <c r="T36" s="106"/>
-      <c r="U36" s="106"/>
-      <c r="V36" s="106"/>
-      <c r="W36" s="106"/>
-      <c r="X36" s="106"/>
-      <c r="Y36" s="106"/>
-      <c r="Z36" s="106"/>
-      <c r="AA36" s="106"/>
-      <c r="AB36" s="106"/>
-      <c r="AC36" s="106"/>
-      <c r="AD36" s="106"/>
-      <c r="AE36" s="106"/>
-      <c r="AF36" s="106"/>
-      <c r="AG36" s="106"/>
-      <c r="AH36" s="106"/>
-      <c r="AI36" s="106"/>
-      <c r="AJ36" s="106"/>
-      <c r="AK36" s="106"/>
-      <c r="AL36" s="106"/>
-      <c r="AM36" s="106"/>
-      <c r="AN36" s="106"/>
-      <c r="AO36" s="106"/>
-      <c r="AP36" s="106"/>
-      <c r="AQ36" s="106"/>
-      <c r="AR36" s="106"/>
-      <c r="AS36" s="106"/>
-      <c r="AT36" s="106"/>
-      <c r="AU36" s="106"/>
-      <c r="AV36" s="106"/>
-      <c r="AW36" s="106"/>
-      <c r="AX36" s="106"/>
-      <c r="AY36" s="106"/>
-      <c r="AZ36" s="106"/>
-      <c r="BA36" s="106"/>
-      <c r="BB36" s="106"/>
-      <c r="BC36" s="106"/>
-      <c r="BD36" s="106"/>
-      <c r="BE36" s="106"/>
-      <c r="BF36" s="106"/>
-      <c r="BG36" s="106"/>
-      <c r="BH36" s="106"/>
-      <c r="BI36" s="106"/>
-      <c r="BJ36" s="106"/>
-      <c r="BK36" s="106"/>
-      <c r="BL36" s="106"/>
-      <c r="BM36" s="106"/>
-      <c r="BN36" s="106"/>
-    </row>
-    <row r="37" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B37" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="80"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="100" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G37" s="61"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="79" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J37" s="98"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="106"/>
-      <c r="N37" s="106"/>
-      <c r="O37" s="106"/>
-      <c r="P37" s="106"/>
-      <c r="Q37" s="106"/>
-      <c r="R37" s="106"/>
-      <c r="S37" s="106"/>
-      <c r="T37" s="106"/>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="106"/>
-      <c r="X37" s="106"/>
-      <c r="Y37" s="106"/>
-      <c r="Z37" s="106"/>
-      <c r="AA37" s="106"/>
-      <c r="AB37" s="106"/>
-      <c r="AC37" s="106"/>
-      <c r="AD37" s="106"/>
-      <c r="AE37" s="106"/>
-      <c r="AF37" s="106"/>
-      <c r="AG37" s="106"/>
-      <c r="AH37" s="106"/>
-      <c r="AI37" s="106"/>
-      <c r="AJ37" s="106"/>
-      <c r="AK37" s="106"/>
-      <c r="AL37" s="106"/>
-      <c r="AM37" s="106"/>
-      <c r="AN37" s="106"/>
-      <c r="AO37" s="106"/>
-      <c r="AP37" s="106"/>
-      <c r="AQ37" s="106"/>
-      <c r="AR37" s="106"/>
-      <c r="AS37" s="106"/>
-      <c r="AT37" s="106"/>
-      <c r="AU37" s="106"/>
-      <c r="AV37" s="106"/>
-      <c r="AW37" s="106"/>
-      <c r="AX37" s="106"/>
-      <c r="AY37" s="106"/>
-      <c r="AZ37" s="106"/>
-      <c r="BA37" s="106"/>
-      <c r="BB37" s="106"/>
-      <c r="BC37" s="106"/>
-      <c r="BD37" s="106"/>
-      <c r="BE37" s="106"/>
-      <c r="BF37" s="106"/>
-      <c r="BG37" s="106"/>
-      <c r="BH37" s="106"/>
-      <c r="BI37" s="106"/>
-      <c r="BJ37" s="106"/>
-      <c r="BK37" s="106"/>
-      <c r="BL37" s="106"/>
-      <c r="BM37" s="106"/>
-      <c r="BN37" s="106"/>
-    </row>
-    <row r="38" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="161" t="str">
+    <row r="36" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="161" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="30"/>
-      <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="30"/>
-      <c r="Z38" s="30"/>
-      <c r="AA38" s="30"/>
-      <c r="AB38" s="30"/>
-      <c r="AC38" s="30"/>
-      <c r="AD38" s="30"/>
-      <c r="AE38" s="30"/>
-      <c r="AF38" s="30"/>
-      <c r="AG38" s="30"/>
-      <c r="AH38" s="30"/>
-      <c r="AI38" s="30"/>
-      <c r="AJ38" s="30"/>
-      <c r="AK38" s="30"/>
-      <c r="AL38" s="30"/>
-      <c r="AM38" s="30"/>
-      <c r="AN38" s="30"/>
-      <c r="AO38" s="30"/>
-      <c r="AP38" s="30"/>
-      <c r="AQ38" s="30"/>
-      <c r="AR38" s="30"/>
-      <c r="AS38" s="30"/>
-      <c r="AT38" s="30"/>
-      <c r="AU38" s="30"/>
-      <c r="AV38" s="30"/>
-      <c r="AW38" s="30"/>
-      <c r="AX38" s="30"/>
-      <c r="AY38" s="30"/>
-      <c r="AZ38" s="30"/>
-      <c r="BA38" s="30"/>
-      <c r="BB38" s="30"/>
-      <c r="BC38" s="30"/>
-      <c r="BD38" s="30"/>
-      <c r="BE38" s="30"/>
-      <c r="BF38" s="30"/>
-      <c r="BG38" s="30"/>
-      <c r="BH38" s="30"/>
-      <c r="BI38" s="30"/>
-      <c r="BJ38" s="30"/>
-      <c r="BK38" s="30"/>
-      <c r="BL38" s="30"/>
-      <c r="BM38" s="30"/>
-      <c r="BN38" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="30"/>
+      <c r="Z36" s="30"/>
+      <c r="AA36" s="30"/>
+      <c r="AB36" s="30"/>
+      <c r="AC36" s="30"/>
+      <c r="AD36" s="30"/>
+      <c r="AE36" s="30"/>
+      <c r="AF36" s="30"/>
+      <c r="AG36" s="30"/>
+      <c r="AH36" s="30"/>
+      <c r="AI36" s="30"/>
+      <c r="AJ36" s="30"/>
+      <c r="AK36" s="30"/>
+      <c r="AL36" s="30"/>
+      <c r="AM36" s="30"/>
+      <c r="AN36" s="30"/>
+      <c r="AO36" s="30"/>
+      <c r="AP36" s="30"/>
+      <c r="AQ36" s="30"/>
+      <c r="AR36" s="30"/>
+      <c r="AS36" s="30"/>
+      <c r="AT36" s="30"/>
+      <c r="AU36" s="30"/>
+      <c r="AV36" s="30"/>
+      <c r="AW36" s="30"/>
+      <c r="AX36" s="30"/>
+      <c r="AY36" s="30"/>
+      <c r="AZ36" s="30"/>
+      <c r="BA36" s="30"/>
+      <c r="BB36" s="30"/>
+      <c r="BC36" s="30"/>
+      <c r="BD36" s="30"/>
+      <c r="BE36" s="30"/>
+      <c r="BF36" s="30"/>
+      <c r="BG36" s="30"/>
+      <c r="BH36" s="30"/>
+      <c r="BI36" s="30"/>
+      <c r="BJ36" s="30"/>
+      <c r="BK36" s="30"/>
+      <c r="BL36" s="30"/>
+      <c r="BM36" s="30"/>
+      <c r="BN36" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7159,18 +6985,9 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H37">
+  <conditionalFormatting sqref="H8:H35">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7189,7 +7006,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN37">
+  <conditionalFormatting sqref="K8:BN35">
     <cfRule type="expression" dxfId="2" priority="48">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
@@ -7197,7 +7014,7 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN37">
+  <conditionalFormatting sqref="K6:BN35">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -7212,8 +7029,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A31:B31 G11:H11 G12 A33:B33 B32 E13 E19 E25 E31:H33 G13:H13 G19:H19 G25:H25 H17 G34 G35:G36 G37 H16 H20:H23 G28:H29 G27 G26" unlockedFormula="1"/>
-    <ignoredError sqref="A25 A19 A13" formula="1"/>
+    <ignoredError sqref="H9 A29:B29 G11:H11 G12 A31:B31 B30 E13 E18 E23 E29:H31 G13:H13 G18:H18 G23:H23 G32 G33:G34 G35 H16 H19:H21 G26:H27 G25 G24" unlockedFormula="1"/>
+    <ignoredError sqref="A23 A18 A13" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -7261,7 +7078,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H37</xm:sqref>
+          <xm:sqref>H8:H35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>